<commit_message>
requirements_artifacts/Melanamo MetaData for Dave Lahr: updated version using correct analyte ID's
</commit_message>
<xml_diff>
--- a/requirements_artifacts/Melanoma MetaData for Dave Lahr.xlsx
+++ b/requirements_artifacts/Melanoma MetaData for Dave Lahr.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\neon-cifs\xchip_prism\PRISM\Cell Team\Melanoma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\neon-cifs\xchip_prism\PRISM\Cell Team\Melanoma\Phase 1 - HTS PRISM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="212">
   <si>
     <t>Pool_ID</t>
   </si>
@@ -71,18 +72,9 @@
     <t>Bin 2</t>
   </si>
   <si>
-    <t>Analyte 111</t>
-  </si>
-  <si>
-    <t>Analyte 120</t>
-  </si>
-  <si>
     <t>Bin 1.5</t>
   </si>
   <si>
-    <t>Analyte 134</t>
-  </si>
-  <si>
     <t>Hs 944.T</t>
   </si>
   <si>
@@ -92,9 +84,6 @@
     <t>HS944T_SKIN</t>
   </si>
   <si>
-    <t>Analyte 136</t>
-  </si>
-  <si>
     <t>LUA-3263</t>
   </si>
   <si>
@@ -107,9 +96,6 @@
     <t>skin</t>
   </si>
   <si>
-    <t>Analyte 145</t>
-  </si>
-  <si>
     <t>M001</t>
   </si>
   <si>
@@ -284,69 +270,9 @@
     <t>LUA-3618</t>
   </si>
   <si>
-    <t>Analyte 376</t>
-  </si>
-  <si>
-    <t>Analyte 54</t>
-  </si>
-  <si>
-    <t>Analyte 239</t>
-  </si>
-  <si>
     <t>Analyte 447</t>
   </si>
   <si>
-    <t>Analyte 260</t>
-  </si>
-  <si>
-    <t>Analyte 196</t>
-  </si>
-  <si>
-    <t>Analyte 385</t>
-  </si>
-  <si>
-    <t>Analyte 180</t>
-  </si>
-  <si>
-    <t>Analyte 173</t>
-  </si>
-  <si>
-    <t>Analyte 159</t>
-  </si>
-  <si>
-    <t>Analyte 318</t>
-  </si>
-  <si>
-    <t>Analyte 426</t>
-  </si>
-  <si>
-    <t>Analyte 178</t>
-  </si>
-  <si>
-    <t>Analyte 79</t>
-  </si>
-  <si>
-    <t>Analyte 355</t>
-  </si>
-  <si>
-    <t>Analyte 63</t>
-  </si>
-  <si>
-    <t>Analyte 153</t>
-  </si>
-  <si>
-    <t>Analyte 187</t>
-  </si>
-  <si>
-    <t>Analyte 235</t>
-  </si>
-  <si>
-    <t>Analyte 184</t>
-  </si>
-  <si>
-    <t>Analyte 65</t>
-  </si>
-  <si>
     <t>MDAMB435S</t>
   </si>
   <si>
@@ -657,6 +583,84 @@
   </si>
   <si>
     <t>Bin 4.5</t>
+  </si>
+  <si>
+    <t>Analyte 458</t>
+  </si>
+  <si>
+    <t>Analyte 452</t>
+  </si>
+  <si>
+    <t>Analyte 466</t>
+  </si>
+  <si>
+    <t>Analyte 454</t>
+  </si>
+  <si>
+    <t>Analyte 456</t>
+  </si>
+  <si>
+    <t>Analyte 459</t>
+  </si>
+  <si>
+    <t>Analyte 449</t>
+  </si>
+  <si>
+    <t>Analyte 446</t>
+  </si>
+  <si>
+    <t>Analyte 453</t>
+  </si>
+  <si>
+    <t>Analyte 462</t>
+  </si>
+  <si>
+    <t>Analyte 443</t>
+  </si>
+  <si>
+    <t>Analyte 460</t>
+  </si>
+  <si>
+    <t>Analyte 461</t>
+  </si>
+  <si>
+    <t>Analyte 450</t>
+  </si>
+  <si>
+    <t>Analyte 455</t>
+  </si>
+  <si>
+    <t>Analyte 463</t>
+  </si>
+  <si>
+    <t>Analyte 469</t>
+  </si>
+  <si>
+    <t>Analyte 451</t>
+  </si>
+  <si>
+    <t>Analyte 467</t>
+  </si>
+  <si>
+    <t>Analyte 457</t>
+  </si>
+  <si>
+    <t>Analyte 444</t>
+  </si>
+  <si>
+    <t>Analyte 465</t>
+  </si>
+  <si>
+    <t>Analyte 448</t>
+  </si>
+  <si>
+    <t>Analyte 464</t>
+  </si>
+  <si>
+    <t>Analyte 468</t>
+  </si>
+  <si>
+    <t>Analyte 445</t>
   </si>
 </sst>
 </file>
@@ -705,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -721,6 +725,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,1028 +1077,1028 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H2">
         <v>445</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>27</v>
+      <c r="I2" t="s">
+        <v>186</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="H3">
         <v>276</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>86</v>
+      <c r="I3" t="s">
+        <v>187</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="H4">
         <v>504</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>87</v>
+      <c r="I4" t="s">
+        <v>188</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H5">
         <v>139</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>88</v>
+      <c r="I5" t="s">
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="H6">
         <v>347</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>89</v>
+      <c r="I6" t="s">
+        <v>189</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="H7">
         <v>411</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>15</v>
+      <c r="I7" t="s">
+        <v>190</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="H8">
         <v>434</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>18</v>
+      <c r="I8" t="s">
+        <v>191</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="M8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="H9">
         <v>160</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>90</v>
+      <c r="I9" t="s">
+        <v>192</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K9" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="M9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="H10">
         <v>96</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>91</v>
+      <c r="I10" t="s">
+        <v>193</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="M10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="H11">
         <v>285</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>92</v>
+      <c r="I11" t="s">
+        <v>194</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="M11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
         <v>112</v>
-      </c>
-      <c r="G12" t="s">
-        <v>137</v>
       </c>
       <c r="H12">
         <v>480</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>93</v>
+      <c r="I12" t="s">
+        <v>195</v>
       </c>
       <c r="J12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K12" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="M12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H13">
         <v>36</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>22</v>
+      <c r="I13" t="s">
+        <v>196</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
         <v>113</v>
-      </c>
-      <c r="G14" t="s">
-        <v>138</v>
       </c>
       <c r="H14">
         <v>473</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>94</v>
+      <c r="I14" t="s">
+        <v>197</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K14" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="M14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
         <v>114</v>
-      </c>
-      <c r="G15" t="s">
-        <v>139</v>
       </c>
       <c r="H15">
         <v>459</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>95</v>
+      <c r="I15" t="s">
+        <v>198</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K15" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="M15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" t="s">
         <v>115</v>
-      </c>
-      <c r="G16" t="s">
-        <v>140</v>
       </c>
       <c r="H16">
         <v>218</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>96</v>
+      <c r="I16" t="s">
+        <v>199</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K16" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="M16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="H17">
         <v>326</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>97</v>
+      <c r="I17" t="s">
+        <v>200</v>
       </c>
       <c r="J17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K17" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="M17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="H18">
         <v>478</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>98</v>
+      <c r="I18" t="s">
+        <v>201</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="M18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="H19">
         <v>529</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>99</v>
+      <c r="I19" t="s">
+        <v>202</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K19" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="M19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="H20">
         <v>255</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>100</v>
+      <c r="I20" t="s">
+        <v>203</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K20" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="M20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="G21" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="H21">
         <v>513</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>101</v>
+      <c r="I21" t="s">
+        <v>204</v>
       </c>
       <c r="J21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="M21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="H22">
         <v>420</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>16</v>
+      <c r="I22" t="s">
+        <v>205</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="M22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
       <c r="D23" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="H23">
         <v>53</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>102</v>
+      <c r="I23" t="s">
+        <v>206</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K23" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="M23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
       <c r="D24" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="H24">
         <v>487</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>103</v>
+      <c r="I24" t="s">
+        <v>207</v>
       </c>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K24" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="M24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="H25">
         <v>135</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>104</v>
+      <c r="I25" t="s">
+        <v>208</v>
       </c>
       <c r="J25" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K25" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="M25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
       <c r="D26" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H26">
         <v>484</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>105</v>
+      <c r="I26" t="s">
+        <v>209</v>
       </c>
       <c r="J26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K26" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="M26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
       <c r="D27" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="H27">
         <v>515</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>106</v>
+      <c r="I27" t="s">
+        <v>210</v>
       </c>
       <c r="J27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="M27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>33</v>
-      </c>
       <c r="D28" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="H28">
         <v>59</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>95</v>
+      <c r="I28" t="s">
+        <v>211</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="M28" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -2107,4 +2114,320 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7">
+        <v>458</v>
+      </c>
+      <c r="E1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7">
+        <v>452</v>
+      </c>
+      <c r="E2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7">
+        <v>466</v>
+      </c>
+      <c r="E3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7">
+        <v>447</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7">
+        <v>454</v>
+      </c>
+      <c r="E5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="7">
+        <v>456</v>
+      </c>
+      <c r="E6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7">
+        <v>459</v>
+      </c>
+      <c r="E7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="7">
+        <v>449</v>
+      </c>
+      <c r="E8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7">
+        <v>446</v>
+      </c>
+      <c r="E9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="7">
+        <v>453</v>
+      </c>
+      <c r="E10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="7">
+        <v>462</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7">
+        <v>443</v>
+      </c>
+      <c r="E12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7">
+        <v>460</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="7">
+        <v>461</v>
+      </c>
+      <c r="E14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="7">
+        <v>450</v>
+      </c>
+      <c r="E15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="7">
+        <v>455</v>
+      </c>
+      <c r="E16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="7">
+        <v>463</v>
+      </c>
+      <c r="E17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="7">
+        <v>469</v>
+      </c>
+      <c r="E18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7">
+        <v>451</v>
+      </c>
+      <c r="E19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="7">
+        <v>467</v>
+      </c>
+      <c r="E20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="7">
+        <v>457</v>
+      </c>
+      <c r="E21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="7">
+        <v>444</v>
+      </c>
+      <c r="E22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="7">
+        <v>465</v>
+      </c>
+      <c r="E23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="7">
+        <v>448</v>
+      </c>
+      <c r="E24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="7">
+        <v>464</v>
+      </c>
+      <c r="E25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="7">
+        <v>468</v>
+      </c>
+      <c r="E26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="7">
+        <v>445</v>
+      </c>
+      <c r="E27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>